<commit_message>
Solved bug coins at 0
</commit_message>
<xml_diff>
--- a/Bot_screening/leaderboards.xlsx
+++ b/Bot_screening/leaderboards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30b5632b4c528d56/Documenti/Arkadia/Coingecko API/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://digitaladvisoryteam82-my.sharepoint.com/personal/davide_galbiati_digitaladvisoryteam82_onmicrosoft_com/Documents/Arkadia_GitHub/Bot_screening/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2C0B9046505C592D5ACD2F7030ABE666F250C478" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01E141A5-C82C-4E91-8E0A-3FAB686083B9}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_0FBF8902CF647336400B70681790EB04E5B95AC0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68218AAE-A54E-4CCE-9629-D5BB3AAC2593}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="1740" windowWidth="16920" windowHeight="10450" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1d" sheetId="1" r:id="rId1"/>
@@ -54,6 +54,27 @@
     <t>polkadot</t>
   </si>
   <si>
+    <t>cardano</t>
+  </si>
+  <si>
+    <t>solana</t>
+  </si>
+  <si>
+    <t>shiba-inu</t>
+  </si>
+  <si>
+    <t>ethereum</t>
+  </si>
+  <si>
+    <t>staked-ether</t>
+  </si>
+  <si>
+    <t>tron</t>
+  </si>
+  <si>
+    <t>dai</t>
+  </si>
+  <si>
     <t>tether</t>
   </si>
   <si>
@@ -63,25 +84,7 @@
     <t>binance-usd</t>
   </si>
   <si>
-    <t>avalanche-2</t>
-  </si>
-  <si>
-    <t>staked-ether</t>
-  </si>
-  <si>
-    <t>ethereum</t>
-  </si>
-  <si>
-    <t>cardano</t>
-  </si>
-  <si>
-    <t>dai</t>
-  </si>
-  <si>
-    <t>matic-network</t>
-  </si>
-  <si>
-    <t>ripple</t>
+    <t>binancecoin</t>
   </si>
   <si>
     <t>dogecoin</t>
@@ -90,13 +93,10 @@
     <t>bitcoin</t>
   </si>
   <si>
-    <t>binancecoin</t>
+    <t>matic-network</t>
   </si>
   <si>
-    <t>shiba-inu</t>
-  </si>
-  <si>
-    <t>solana</t>
+    <t>ripple</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -475,7 +477,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>2.3527025656627051E-2</v>
+        <v>3.2619957994466507E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -483,7 +485,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2.2644927536231828E-2</v>
+        <v>2.2036522101481701E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -491,7 +493,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2.2644927536231828E-2</v>
+        <v>2.0411814488952171E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -499,7 +501,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2.1739130434782549E-2</v>
+        <v>8.7688663992207677E-3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -507,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>9.0978811443246412E-3</v>
+        <v>8.08520044723985E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -515,7 +517,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>8.1246947439256208E-3</v>
+        <v>7.7158088753957743E-3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -523,7 +525,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>7.806753599194402E-3</v>
+        <v>4.5478141977180597E-3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -531,7 +533,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2.164502164502168E-3</v>
+        <v>2.4396165504958389E-3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -539,7 +541,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.811594202898552E-3</v>
+        <v>2.3586099889643581E-3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -547,7 +549,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>7.1123755334282293E-4</v>
+        <v>2.3586099889643581E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -555,7 +557,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>2.3586099889643581E-3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -563,7 +565,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>-1.9462479989380401E-4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -571,7 +573,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-1.7403416570620151E-3</v>
+        <v>-1.0688020556503979E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -579,7 +581,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-3.9332282128413587E-3</v>
+        <v>-2.3586099889643581E-3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -587,7 +589,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-1.1148939747388731E-2</v>
+        <v>-3.0005435457452659E-3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -595,7 +597,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>-1.9551543797551921E-2</v>
+        <v>-1.054641132174221E-2</v>
       </c>
     </row>
   </sheetData>
@@ -618,130 +620,130 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0.18667686377841691</v>
+        <v>0.1450702662276947</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>0.1186443738263757</v>
+        <v>0.12805425553441349</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>0.1186443738263757</v>
+        <v>0.1029819156008738</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>0.11773857672492639</v>
+        <v>0.10266018157417529</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>8.3333333333333315E-2</v>
+        <v>0.1020357215419667</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>7.4001516683518509E-2</v>
+        <v>0.1008976991753892</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B8">
-        <v>2.4948491234341692E-2</v>
+        <v>8.1540211643570198E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>4.6273364309307868E-3</v>
+        <v>6.8997129395750395E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B10">
-        <v>-3.5361377752682131E-2</v>
+        <v>5.8797159268247218E-5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>-4.2313374399665121E-2</v>
+        <v>-1.746250892758156E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>-4.4645354760568197E-2</v>
+        <v>-1.1090425079668139E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>-6.2499999999999931E-2</v>
+        <v>-1.523769551204663E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>-7.5758564363568009E-2</v>
+        <v>-1.7072576448359279E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>-8.3610078478146638E-2</v>
+        <v>-4.054929451507383E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>-0.10506858174912879</v>
+        <v>-4.2278114712809192E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.11854188103812489</v>
+        <v>-9.9663277228582745E-2</v>
       </c>
     </row>
   </sheetData>
@@ -764,130 +766,130 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0.1925134396539033</v>
+        <v>0.15381259024570099</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>0.1186443738263757</v>
+        <v>0.1119323516990354</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>0.1186443738263757</v>
+        <v>0.11161061767233681</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>0.11773857672492639</v>
+        <v>0.1109861576401283</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>8.3333333333333315E-2</v>
+        <v>0.1098481352735507</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>7.4001516683518509E-2</v>
+        <v>0.1076907334706964</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>2.0350449110342912E-2</v>
+        <v>7.5077248843021915E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B9">
-        <v>4.6273364309307938E-3</v>
+        <v>7.1010128261212224E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>-2.9908453270459951E-2</v>
+        <v>4.3595398308429352E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>-3.1722771823115108E-2</v>
+        <v>1.421751052350767E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>-3.5361377752682097E-2</v>
+        <v>4.6882343942012492E-3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>-6.2499999999999931E-2</v>
+        <v>3.9127799554300388E-3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>-7.0181319522519603E-2</v>
+        <v>3.5081056039031212E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>-7.3220468088536134E-2</v>
+        <v>-1.062532724056906E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-0.103028767552022</v>
+        <v>-4.0780828366828767E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.1118473203686689</v>
+        <v>-0.1086137133267443</v>
       </c>
     </row>
   </sheetData>
@@ -910,106 +912,106 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0.18093042807089171</v>
+        <v>0.15182760575800569</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>9.4834850016851963E-2</v>
+        <v>0.1054770858236713</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>9.4834850016851963E-2</v>
+        <v>0.1051553517969728</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>9.3929052915402683E-2</v>
+        <v>0.1045308917647642</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>8.3333333333333315E-2</v>
+        <v>0.10339286939818659</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>5.0191992873994763E-2</v>
+        <v>0.1019098681916952</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B8">
-        <v>-2.8649989261075172E-3</v>
+        <v>7.1107942333423518E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>-1.041947986412973E-2</v>
+        <v>5.4228717929411453E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>-1.6159848903103399E-2</v>
+        <v>3.7140132433065277E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>-2.101368921009478E-2</v>
+        <v>9.3317508697994683E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>-3.5361377752682097E-2</v>
+        <v>9.0521526022926384E-3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>-4.5024086818116968E-2</v>
+        <v>7.2937351775593752E-3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>-6.2499999999999931E-2</v>
+        <v>2.4571239371002991E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -1017,23 +1019,23 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>-8.1361463491427796E-2</v>
+        <v>-6.1326469506336988E-3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-0.1227254185835856</v>
+        <v>-3.5968488608390012E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.12993942563182689</v>
+        <v>-0.10215844745138029</v>
       </c>
     </row>
   </sheetData>
@@ -1056,90 +1058,90 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0.2296119696530419</v>
+        <v>0.15370332916200249</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>8.3333333333333315E-2</v>
+        <v>0.1281593072642582</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>7.1579036063363494E-2</v>
+        <v>0.10777480799059611</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>7.1579036063363494E-2</v>
+        <v>8.0947845778479605E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>7.0673238961914214E-2</v>
+        <v>8.0626111751781054E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>4.0105612611670637E-2</v>
+        <v>7.8874651719572503E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>3.3117453755439147E-2</v>
+        <v>7.8863629352994902E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>2.6936178920506312E-2</v>
+        <v>5.3747512212094208E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>5.3021002635893558E-3</v>
+        <v>4.716808747087585E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>-1.927724232524311E-3</v>
+        <v>4.0400951268400903E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B12">
-        <v>-3.5361377752682097E-2</v>
+        <v>1.261089238787355E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -1147,7 +1149,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-3.7561400250952788E-2</v>
+        <v>1.018441086370348E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -1155,31 +1157,31 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-6.1092702034098792E-2</v>
+        <v>-1.294169021763613E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B15">
-        <v>-6.2499999999999931E-2</v>
+        <v>-6.0988181165662061E-3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-6.4830681741480378E-2</v>
+        <v>-3.1213878262164031E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.108913353302138</v>
+        <v>-7.7629207406188505E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1202,90 +1204,90 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0.19866419402441521</v>
+        <v>0.13488237589688079</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>9.5388559872887399E-2</v>
+        <v>0.1133486079620518</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>9.5388559872887399E-2</v>
+        <v>0.1044430413053639</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>9.448276277143812E-2</v>
+        <v>0.1038303072786653</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>8.3333333333333315E-2</v>
+        <v>0.102662933120618</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>5.0745702730030207E-2</v>
+        <v>9.8795824879879257E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B8">
-        <v>2.2052357597264149E-2</v>
+        <v>9.6323766958340551E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>1.5835433662212552E-2</v>
+        <v>6.3998477465153317E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>1.071747522935501E-2</v>
+        <v>3.6106087914757883E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>-2.0338925377436218E-2</v>
+        <v>2.8535157382481569E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>-3.5361377752682097E-2</v>
+        <v>2.4578198012419991E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -1293,39 +1295,39 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-5.7843090391797858E-2</v>
+        <v>3.8129103775440699E-3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>-6.2499999999999931E-2</v>
+        <v>2.7663955630399199E-4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>-8.2871918854882459E-2</v>
+        <v>-2.0717736974390451E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-9.8339044619003155E-2</v>
+        <v>-6.7608792625389588E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.11559672840656569</v>
+        <v>-0.1011244029330728</v>
       </c>
     </row>
   </sheetData>
@@ -1348,58 +1350,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0.19097188633210771</v>
+        <v>0.16625284499278711</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>8.3333333333333315E-2</v>
+        <v>0.14441537314290889</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>7.2132745919398916E-2</v>
+        <v>0.1121780691310838</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>7.2132745919398916E-2</v>
+        <v>8.121656091728427E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>7.1226948817949637E-2</v>
+        <v>8.0523770290569521E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>2.7489888776541731E-2</v>
+        <v>8.0050878103009607E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>2.6987886373787379E-2</v>
+        <v>7.5489287891783413E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1407,71 +1409,71 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>1.4448008627803091E-2</v>
+        <v>5.2790320213037138E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>-7.7860482447374389E-3</v>
+        <v>4.357956304230446E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>-3.5361377752682097E-2</v>
+        <v>4.1839338961842359E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>-4.5338925377436293E-2</v>
+        <v>3.9195104428299883E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>-4.9870425243734029E-2</v>
+        <v>1.279955092666207E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>-5.9062395045358797E-2</v>
+        <v>3.3867643369265392E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>-6.2499999999999931E-2</v>
+        <v>-3.3944713797838928E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-6.4649661833253907E-2</v>
+        <v>-3.5295399138398673E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.1205842595786356</v>
+        <v>-7.7817865944976986E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1494,58 +1496,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0.1928986686057107</v>
+        <v>0.1251126929687526</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>8.3333333333333315E-2</v>
+        <v>0.1192152546491362</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>7.213274591939893E-2</v>
+        <v>8.9612025825781344E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>7.213274591939893E-2</v>
+        <v>8.891923519906661E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>7.1226948817949637E-2</v>
+        <v>8.8701024079421459E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>2.7489888776541731E-2</v>
+        <v>8.8446343011506667E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>1.9638753571458091E-2</v>
+        <v>8.3231752800280473E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1553,71 +1555,71 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>9.3496246937980476E-3</v>
+        <v>6.6080201177681444E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>2.825959314500848E-3</v>
+        <v>3.5025285503356159E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <v>-3.5361377752682097E-2</v>
+        <v>-3.838132231918593E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>-4.2933362787294163E-2</v>
+        <v>-1.771441728243648E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B13">
-        <v>-4.5338925377436307E-2</v>
+        <v>-2.6164468040694531E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>-5.2147033098031183E-2</v>
+        <v>-4.4741874354887877E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>-6.2499999999999931E-2</v>
+        <v>-5.0233555593412353E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-6.3592764295010734E-2</v>
+        <v>-6.8901004320859341E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-6.9973439334307636E-2</v>
+        <v>-8.6213330853474074E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1640,130 +1642,130 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>0.18716253093840671</v>
+        <v>0.17460997050360899</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>8.3333333333333315E-2</v>
+        <v>0.17391717987689431</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>4.9405473192126251E-2</v>
+        <v>0.17365333137946559</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>4.9405473192126251E-2</v>
+        <v>0.16905738197318571</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>4.8499676090676971E-2</v>
+        <v>0.100847030063572</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>2.8773687989123609E-2</v>
+        <v>9.2490239879685077E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>1.912608673204319E-2</v>
+        <v>9.1102376299243754E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B9">
-        <v>1.706921007295786E-2</v>
+        <v>6.6556111614392011E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>1.362021210423176E-2</v>
+        <v>6.1693186754417317E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>4.7626160492690653E-3</v>
+        <v>3.4764389084415398E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>-1.9697899736410559E-2</v>
+        <v>-2.0663615197190649E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>-3.5361377752682097E-2</v>
+        <v>-2.3819774284823299E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>-3.755701870127269E-2</v>
+        <v>-3.279668726849759E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>-4.5836074979844182E-2</v>
+        <v>-6.8054887355106508E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-5.2176252772451401E-2</v>
+        <v>-7.2275152666287409E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-6.2499999999999931E-2</v>
+        <v>-0.1712112755313018</v>
       </c>
     </row>
   </sheetData>
@@ -1786,34 +1788,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>0.19100130253149691</v>
+        <v>0.17487572486847169</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>8.3333333333333315E-2</v>
+        <v>0.17472840437544521</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>5.18942368483261E-2</v>
+        <v>0.17404419500216001</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>4.8499676090676958E-2</v>
+        <v>0.16986860647173649</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1821,15 +1823,15 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>4.7940555928063178E-2</v>
+        <v>9.4359516180374067E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>4.2404457246107141E-2</v>
+        <v>7.7849158695617454E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1837,39 +1839,39 @@
         <v>1</v>
       </c>
       <c r="B8">
-        <v>2.7183250969903941E-2</v>
+        <v>7.14126054058844E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B9">
-        <v>2.7183250969903941E-2</v>
+        <v>5.9063658770119577E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>1.136550267081831E-2</v>
+        <v>4.4370956813678038E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>1.033030524238922E-2</v>
+        <v>-9.7154721781575713E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>-1.7459606172953251E-2</v>
+        <v>-1.9831512736185782E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -1877,39 +1879,39 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-3.004660129563359E-2</v>
+        <v>-2.8462496243568822E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B14">
-        <v>-3.5361377752682131E-2</v>
+        <v>-3.109105308370046E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>-3.8479903060734753E-2</v>
+        <v>-7.8566548789828133E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B16">
-        <v>-4.4697899736410668E-2</v>
+        <v>-0.11657374072057899</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-6.2499999999999931E-2</v>
+        <v>-0.1720225000298527</v>
       </c>
     </row>
   </sheetData>
@@ -1932,50 +1934,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>0.2066263025314968</v>
+        <v>0.19212015565866339</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>8.3333333333333315E-2</v>
+        <v>0.19197283516563701</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>7.1755490044165274E-2</v>
+        <v>0.1912886257923517</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>5.4277368923249407E-2</v>
+        <v>0.18711303726192829</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>5.4164047675074913E-2</v>
+        <v>0.10655691783544299</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>5.2703743294275567E-2</v>
+        <v>6.4854447650697283E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1983,79 +1985,79 @@
         <v>1</v>
       </c>
       <c r="B8">
-        <v>5.0439064923392243E-2</v>
+        <v>5.4979794052174673E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>5.0439064923392243E-2</v>
+        <v>4.632041309549384E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>4.7292042778853988E-2</v>
+        <v>3.6804703555796701E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <v>5.7962077805350579E-3</v>
+        <v>-2.90461481216021E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>4.7280643460306943E-3</v>
+        <v>-3.6911631608513669E-3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B13">
-        <v>-1.9056874095384931E-2</v>
+        <v>-1.2568858636575369E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B14">
-        <v>-3.2384415439409203E-2</v>
+        <v>-1.384662229350871E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>-3.5361377752682097E-2</v>
+        <v>-9.8136195332352183E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B16">
-        <v>-6.2499999999999931E-2</v>
+        <v>-0.12606496175822099</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-7.6275104314068295E-2</v>
+        <v>-0.18926693082004439</v>
       </c>
     </row>
   </sheetData>
@@ -2078,10 +2080,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>4.9783549783549819E-2</v>
+        <v>9.6860263146351724E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2089,95 +2091,95 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>4.1174084480156407E-2</v>
+        <v>3.4795012051151132E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>3.7486446132472692E-2</v>
+        <v>3.016750207727778E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>3.4049896499410988E-2</v>
+        <v>2.5783296703001699E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>2.7738264580369959E-2</v>
+        <v>1.891330543674509E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>2.1738675626420581E-2</v>
+        <v>1.8456807352886941E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>2.1566195331033811E-2</v>
+        <v>1.368740468087117E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>1.99720083468558E-2</v>
+        <v>1.28028100937147E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>1.7043431728564911E-2</v>
+        <v>1.0551877368171409E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>1.0843592980563531E-2</v>
+        <v>9.3844715145324289E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>1.8115942028984131E-3</v>
+        <v>7.9175581329266054E-3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>1.8115942028984131E-3</v>
+        <v>7.8385198986325316E-3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>9.0579710144913367E-4</v>
+        <v>7.3581548321462334E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -2185,23 +2187,23 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>6.7421482706147987E-3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>6.1219052948211471E-3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-1.902173913043486E-2</v>
+        <v>-7.2771482706147509E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2224,42 +2226,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>0.20274280738586581</v>
+        <v>0.2027251389189455</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>9.4578638708338603E-2</v>
+        <v>0.20250838951055089</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>8.3333333333333315E-2</v>
+        <v>0.2020409295456603</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>7.1755490044165288E-2</v>
+        <v>0.19414333357122199</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>6.3180821329002892E-2</v>
+        <v>0.1231246889960947</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -2267,63 +2269,63 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <v>5.0439064923392257E-2</v>
+        <v>6.9142754940998585E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B8">
-        <v>5.0439064923392257E-2</v>
+        <v>4.9475707385080163E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>4.5700942173827377E-2</v>
+        <v>4.2009350076262338E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>4.5674508005227918E-2</v>
+        <v>4.1881638410126779E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <v>3.362979845007686E-2</v>
+        <v>6.9680803536020103E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B12">
-        <v>7.2589153782992299E-3</v>
+        <v>-3.0943185402001329E-3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>5.7962077805350856E-3</v>
+        <v>-7.5167807997580998E-3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>-3.5361377752682097E-2</v>
+        <v>-1.8718832333907601E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -2331,23 +2333,23 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>-5.4459562388407809E-2</v>
+        <v>-1.9757676741183269E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-6.2499999999999931E-2</v>
+        <v>-0.1094494056827742</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-7.6977503510758133E-2</v>
+        <v>-0.20001923457335299</v>
       </c>
     </row>
   </sheetData>
@@ -2370,34 +2372,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>0.20080482288974169</v>
+        <v>0.2099359566261671</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>0.1148411489626455</v>
+        <v>0.2097192072177724</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>8.3333333333333315E-2</v>
+        <v>0.2092517472528819</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>6.6151118358705838E-2</v>
+        <v>0.20135415127844361</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -2405,95 +2407,95 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>5.540295187583695E-2</v>
+        <v>0.1059204363703834</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>5.1995455567458881E-2</v>
+        <v>5.9503551515543651E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>4.9028217316892622E-2</v>
+        <v>4.734264486205831E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9">
-        <v>2.7711792196119588E-2</v>
+        <v>3.3484875292376128E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B10">
-        <v>2.7711792196119588E-2</v>
+        <v>1.751245311114465E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <v>2.8174735201048772E-3</v>
+        <v>-6.8223652718006483E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>-1.6931064946737601E-2</v>
+        <v>-1.8367010881428059E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B13">
-        <v>-1.8382110262726369E-2</v>
+        <v>-2.953076735664208E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>-3.5361377752682097E-2</v>
+        <v>-4.6419526568522489E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>-4.8295926230615252E-2</v>
+        <v>-5.4707030244743327E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-6.2499999999999931E-2</v>
+        <v>-0.1292357112329105</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-7.2510725174633084E-2</v>
+        <v>-0.20723005228057459</v>
       </c>
     </row>
   </sheetData>
@@ -2516,130 +2518,130 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>0.22258700110756341</v>
+        <v>0.21707540780943479</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>0.11656798063767219</v>
+        <v>0.21685865840104021</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>9.664726493594028E-2</v>
+        <v>0.2163911984361496</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>8.3333333333333315E-2</v>
+        <v>0.20849360246171131</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>7.533083981516725E-2</v>
+        <v>0.18320165170775521</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>7.533083981516725E-2</v>
+        <v>0.1230737441026562</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>4.0064161836966788E-2</v>
+        <v>8.631577768475307E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B9">
-        <v>3.8640772237444901E-2</v>
+        <v>4.442143980732919E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>3.6330216462696643E-2</v>
+        <v>3.7538676611131742E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>3.0687982672310061E-2</v>
+        <v>1.326972607659054E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>-3.5361377752682097E-2</v>
+        <v>1.7887233252815991E-3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>-4.3382110262726453E-2</v>
+        <v>-3.0391453028438889E-3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>-6.050706473847027E-2</v>
+        <v>-3.6788436935367319E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B15">
-        <v>-6.2499999999999931E-2</v>
+        <v>-4.7589677424217033E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-8.7775952754057515E-2</v>
+        <v>-0.1532522548927884</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-9.9743840643042619E-2</v>
+        <v>-0.21436950346384229</v>
       </c>
     </row>
   </sheetData>
@@ -2662,50 +2664,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>0.22258700110756349</v>
+        <v>0.2069417979623375</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>0.12562296911314139</v>
+        <v>0.20685754737073209</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>9.6647264935940266E-2</v>
+        <v>0.20647433799744691</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>8.3333333333333315E-2</v>
+        <v>0.19927856104580821</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>7.5330839815167236E-2</v>
+        <v>0.1732847912690525</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>7.5330839815167236E-2</v>
+        <v>0.1086911962112881</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -2713,79 +2715,79 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>5.6889154573691862E-2</v>
+        <v>0.1082490652959099</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>4.944013137848069E-2</v>
+        <v>9.1319843147132929E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>3.9096107625930833E-2</v>
+        <v>6.2379823033343947E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>3.0687982672310061E-2</v>
+        <v>3.007957346889609E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>7.6747534433478579E-3</v>
+        <v>-1.4660053900808661E-3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>-1.7741084621700699E-2</v>
+        <v>-1.1894434616281211E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>-3.5361377752682097E-2</v>
+        <v>-1.8519486720912089E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B15">
-        <v>-6.2499999999999931E-2</v>
+        <v>-2.3017878102185099E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-0.1104840816993657</v>
+        <v>-0.1185802737451143</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.1216455500447521</v>
+        <v>-0.2044526430251396</v>
       </c>
     </row>
   </sheetData>
@@ -2808,42 +2810,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>0.25313689927456973</v>
+        <v>0.25457831040527901</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>9.9510783426487476E-2</v>
+        <v>0.20498876241962649</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>8.3333333333333315E-2</v>
+        <v>0.20443452380034019</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>7.2837741126416514E-2</v>
+        <v>0.20239506121773321</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>5.373025396739408E-2</v>
+        <v>0.19753683567917299</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -2851,87 +2853,87 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <v>5.1521316005643497E-2</v>
+        <v>0.1094469002214643</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>5.1521316005643497E-2</v>
+        <v>0.10178673026192619</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>3.6744520885208229E-2</v>
+        <v>8.6025033443581422E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>3.3099105912228768E-2</v>
+        <v>6.6015552276511236E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>2.5755321540175079E-2</v>
+        <v>2.310110896504082E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B12">
-        <v>6.8784588627863116E-3</v>
+        <v>-1.03102300693643E-3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>4.1666666666666657E-3</v>
+        <v>-1.1570548734169069E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>-1.774108462170073E-2</v>
+        <v>-1.3793027031647431E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>-3.5361377752682097E-2</v>
+        <v>-1.65671319118493E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-5.2581623104112747E-2</v>
+        <v>-0.1139303532248047</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-8.3250693881667587E-2</v>
+        <v>-0.2024128288280328</v>
       </c>
     </row>
   </sheetData>
@@ -2954,74 +2956,74 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>0.23513689927456949</v>
+        <v>0.23291100634468481</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>0.16998434505850679</v>
+        <v>0.18276045835903221</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>8.3333333333333315E-2</v>
+        <v>0.1826672197397459</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>7.6019445356507315E-2</v>
+        <v>0.179990757157139</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>7.4563587300727374E-2</v>
+        <v>0.17513753161857881</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>7.2837741126416514E-2</v>
+        <v>9.3145412124879368E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>5.1521316005643497E-2</v>
+        <v>8.8844680807122114E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>5.1521316005643497E-2</v>
+        <v>7.091010983845808E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>2.8447750532114961E-2</v>
+        <v>5.8038309771437681E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -3029,55 +3031,55 @@
         <v>5</v>
       </c>
       <c r="B11">
-        <v>2.131856306710047E-2</v>
+        <v>5.4979246362752386E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>6.8784588627863116E-3</v>
+        <v>1.815097197825417E-3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>-1.7741084621700709E-2</v>
+        <v>-1.2268269191566079E-3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>-3.5361377752682097E-2</v>
+        <v>-3.058020345257147E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B15">
-        <v>-5.3147233963841342E-2</v>
+        <v>-5.2017698795279482E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-5.8333333333333258E-2</v>
+        <v>-8.8934214345360252E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-7.7787939779559473E-2</v>
+        <v>-0.1807455247674386</v>
       </c>
     </row>
   </sheetData>
@@ -3100,130 +3102,130 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>0.24323406526647259</v>
+        <v>0.30355133579644672</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>0.15266685779195319</v>
+        <v>0.17249169690170321</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>0.1231892566772621</v>
+        <v>0.1623204582824169</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>8.3333333333333315E-2</v>
+        <v>0.15972199569980999</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>7.5555650792790793E-2</v>
+        <v>0.1504727701612498</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>6.7094677714073833E-2</v>
+        <v>0.1078078272326907</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B8">
-        <v>4.6675648607142052E-2</v>
+        <v>8.7485137384314765E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>3.4890494325667737E-2</v>
+        <v>7.8099453188732584E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>2.7383195671871041E-2</v>
+        <v>5.6957775518205363E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>6.0667705510979927E-3</v>
+        <v>5.4533946827810549E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>6.0667705510979927E-3</v>
+        <v>5.1260729514245248E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>-3.1978900582360477E-2</v>
+        <v>6.2118332627500404E-3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>-3.5259178568573017E-2</v>
+        <v>-6.6225504315224181E-4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>-3.8576086591759193E-2</v>
+        <v>-2.4488902210374058E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-8.0815923207227608E-2</v>
+        <v>-8.1880571431104512E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.1208333333333332</v>
+        <v>-0.1604767633101096</v>
       </c>
     </row>
   </sheetData>
@@ -3246,66 +3248,66 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>0.2472420812985367</v>
+        <v>0.34079767838135111</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>0.17153315689601939</v>
+        <v>0.20973803948660749</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>0.14880405843610281</v>
+        <v>0.19956680086732129</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>0.13784672422926009</v>
+        <v>0.19696833828471441</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>0.12953846302646849</v>
+        <v>0.18771911274615419</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>0.1206047800399536</v>
+        <v>9.1316456474268407E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>0.1164525122321734</v>
+        <v>8.8503455875314066E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>8.3333333333333315E-2</v>
+        <v>7.8673151682484843E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -3313,63 +3315,63 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>4.280453230201773E-2</v>
+        <v>7.362795777701342E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>-8.3613901645085524E-3</v>
+        <v>3.8444882907267927E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>-5.595013766146234E-2</v>
+        <v>3.0165014423314429E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>-7.7266562782235371E-2</v>
+        <v>1.6065794858825221E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B14">
-        <v>-7.7266562782235371E-2</v>
+        <v>-8.2102848627868055E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>-8.0815923207227608E-2</v>
+        <v>-2.8919034059888521E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-0.1208333333333332</v>
+        <v>-0.10102520628980929</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.12190941992509249</v>
+        <v>-0.19772310589501399</v>
       </c>
     </row>
   </sheetData>
@@ -3392,66 +3394,66 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>0.23728192193598691</v>
+        <v>0.30710829559560188</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>0.17698298388563871</v>
+        <v>0.17632173125021031</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>0.1169598466742673</v>
+        <v>0.165877418081572</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>0.10933037422557659</v>
+        <v>0.16283995549896521</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>0.1019830151319452</v>
+        <v>0.15493855517369859</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>8.3333333333333315E-2</v>
+        <v>7.8708818815863696E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>7.8822683344778807E-2</v>
+        <v>6.3109185443651641E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>6.6550725985899492E-2</v>
+        <v>4.8915746445676117E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -3459,63 +3461,63 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>2.8208785564138509E-3</v>
+        <v>4.8434996413766633E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>-1.2471876791897089E-2</v>
+        <v>4.3203506139256387E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>-3.3788301912670099E-2</v>
+        <v>3.3105646844022153E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>-3.3788301912670099E-2</v>
+        <v>1.7461062945071229E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>-3.9449473066062953E-2</v>
+        <v>-8.2346439507218171E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>-7.8431159055527305E-2</v>
+        <v>-4.8461118662482323E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-8.0815923207227608E-2</v>
+        <v>-9.3712870440645649E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.1208333333333332</v>
+        <v>-0.1640337231092647</v>
       </c>
     </row>
   </sheetData>
@@ -3538,106 +3540,106 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>0.23728192193598691</v>
+        <v>0.30605139805735881</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>0.1888526771796952</v>
+        <v>0.17526483371196711</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>0.1046899080239606</v>
+        <v>0.16482052054332891</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>8.3639073310876513E-2</v>
+        <v>0.16178305796072201</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>8.3333333333333315E-2</v>
+        <v>0.1538816576354555</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>5.9504173382318448E-2</v>
+        <v>8.09946072037004E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>5.8048322943525452E-2</v>
+        <v>6.4625738473712349E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>4.0909700344873963E-2</v>
+        <v>4.8323365092612758E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>3.2982668662648387E-2</v>
+        <v>4.4534374458271679E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>1.1666243541875371E-2</v>
+        <v>3.5800657764035411E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B12">
-        <v>1.1666243541875371E-2</v>
+        <v>3.2626645128728267E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>-3.2539862634656552E-2</v>
+        <v>2.8137649593136971E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>-3.2976613600981829E-2</v>
+        <v>2.4871691181398048E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -3645,23 +3647,23 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>-5.8380430749804667E-2</v>
+        <v>-4.9888321449469378E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-0.1208333333333332</v>
+        <v>-9.5505964297907281E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.12429418407679289</v>
+        <v>-0.16297682557102161</v>
       </c>
     </row>
   </sheetData>
@@ -3684,10 +3686,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>2.794773236840685E-2</v>
+        <v>9.4509378038238168E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -3695,119 +3697,119 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>1.5605902661974581E-2</v>
+        <v>7.5839244043265669E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>1.317073042253674E-2</v>
+        <v>2.9105917735401009E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B5">
-        <v>8.0275916666974166E-3</v>
+        <v>2.0057441414629E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>4.3290043290043351E-3</v>
+        <v>1.977378654420929E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>1.8115942028984131E-3</v>
+        <v>1.570666687156335E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>1.8115942028984131E-3</v>
+        <v>1.517743759405585E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>9.0579710144913367E-4</v>
+        <v>1.4802728200441279E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>7.1123755334300681E-4</v>
+        <v>1.4628353246810119E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>6.5046863183757936E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>7.6684079446403489E-4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>-1.902173913043486E-2</v>
+        <v>6.558015361371617E-4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>-2.3540361174164231E-2</v>
+        <v>1.754364696508618E-4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>-2.884264422080219E-2</v>
+        <v>-9.4429908119380082E-5</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B16">
-        <v>-4.0107528981743787E-2</v>
+        <v>-4.405700918805721E-4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>-4.0853200582476892E-2</v>
+        <v>-4.384723100913368E-3</v>
       </c>
     </row>
   </sheetData>
@@ -3830,106 +3832,106 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>0.23922744722781569</v>
+        <v>0.30734245794168058</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>0.18755644489486961</v>
+        <v>0.17560789359628901</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>0.10163180404842551</v>
+        <v>0.16566658042765059</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>8.3333333333333315E-2</v>
+        <v>0.16241001424488219</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>8.0560491444716872E-2</v>
+        <v>0.15450771751977729</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>5.9951272515361628E-2</v>
+        <v>8.1416448787026044E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>5.7421954662593852E-2</v>
+        <v>6.0725993498071791E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B9">
-        <v>4.0909700344873963E-2</v>
+        <v>4.2129159270960372E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B10">
-        <v>3.298266866264838E-2</v>
+        <v>4.0452577879657517E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>1.166624354187535E-2</v>
+        <v>3.7664904567628291E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>1.166624354187535E-2</v>
+        <v>2.770307387806276E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>-3.2976613600981829E-2</v>
+        <v>2.4774847870192969E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>-3.6931820557403343E-2</v>
+        <v>2.3363665310114939E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -3937,23 +3939,23 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>-6.0046172004663202E-2</v>
+        <v>-5.0708786283033949E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>-0.1208333333333332</v>
+        <v>-9.1500865430116388E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.12429418407679289</v>
+        <v>-0.1642678854553434</v>
       </c>
     </row>
   </sheetData>
@@ -3965,12 +3967,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
@@ -3982,127 +3981,127 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>9.4834850016851796E-2</v>
+        <v>0.1134664666595937</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>9.4834850016851796E-2</v>
+        <v>8.460695437196096E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>9.3929052915402517E-2</v>
+        <v>6.5133253375693284E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>7.4001516683518509E-2</v>
+        <v>3.3655631684358582E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>5.7255424676099231E-2</v>
+        <v>2.513155157664845E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>3.890580001783796E-3</v>
+        <v>2.4140844665003169E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>2.18304273216063E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>2.1402734154079929E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>-6.6782199006994516E-3</v>
+        <v>2.1206065954538961E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>-1.0422592835147459E-2</v>
+        <v>2.0977534510585621E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>-2.560455192034131E-2</v>
+        <v>1.8251299391666718E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B13">
-        <v>-2.6974820246860369E-2</v>
+        <v>1.7606183816650869E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>-3.9149256540560923E-2</v>
+        <v>8.5414921694124523E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>-4.668836588437987E-2</v>
+        <v>8.466017010001381E-3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B16">
-        <v>-4.7963148092070147E-2</v>
+        <v>8.2046235727931439E-3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-7.1827214255290997E-2</v>
+        <v>-1.8721295166392041E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4128,127 +4127,127 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>9.4834850016851796E-2</v>
+        <v>0.1117077240543969</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>9.4834850016851796E-2</v>
+        <v>8.5434054289299413E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>9.3929052915402517E-2</v>
+        <v>7.5815637580034984E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>7.4001516683518509E-2</v>
+        <v>2.9036928677698009E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>4.0616489567946182E-2</v>
+        <v>2.45381969485324E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>2.4367617382645038E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>-1.4965512718379049E-2</v>
+        <v>2.2632709003959441E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>-3.2295778636440023E-2</v>
+        <v>2.0809379525963869E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>-3.325335905964584E-2</v>
+        <v>2.0612711326422901E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>-3.536449766886457E-2</v>
+        <v>2.0384179882469562E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>-3.9149256540560923E-2</v>
+        <v>1.7657944763550659E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>-4.8678820593154627E-2</v>
+        <v>1.110869379919772E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>-5.1245577561366877E-2</v>
+        <v>6.2837778642078554E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15">
-        <v>-7.0351844240640504E-2</v>
+        <v>-3.264053254397751E-3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B16">
-        <v>-7.2638438753841836E-2</v>
+        <v>-5.5609845736651854E-3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.24999999999999989</v>
+        <v>-1.8127940538275981E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4274,127 +4273,127 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.1186443738263757</v>
+        <v>0.11891768281367231</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>0.1186443738263757</v>
+        <v>8.4622737728099362E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>0.11773857672492639</v>
+        <v>7.3462861212051908E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>7.4001516683518509E-2</v>
+        <v>4.0461006660685188E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>4.1829897728116093E-2</v>
+        <v>3.7009265988376457E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>3.6756569890371973E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>-2.644886832727986E-2</v>
+        <v>3.6306989594622363E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>-2.8286429195105871E-2</v>
+        <v>3.543117219723517E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>-3.9289837042703377E-2</v>
+        <v>3.5040039026935067E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>-5.1245577561366877E-2</v>
+        <v>2.3917334893250718E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>-5.3774712359701257E-2</v>
+        <v>2.3697646261304162E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>-6.1813671731508438E-2</v>
+        <v>1.499094584341645E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>-8.0815923207227608E-2</v>
+        <v>1.244185751131417E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15">
-        <v>-8.9639678068533762E-2</v>
+        <v>5.3662375149923832E-3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>-8.9882869544033614E-2</v>
+        <v>3.976979300966306E-3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.24999999999999989</v>
+        <v>-3.405075025042878E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4406,9 +4405,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
@@ -4420,127 +4422,127 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.1186443738263757</v>
+        <v>0.1176834665204357</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>0.1186443738263757</v>
+        <v>7.7469154192916223E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>0.11773857672492639</v>
+        <v>6.4446777587131771E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>8.3333333333333315E-2</v>
+        <v>4.7266675984516088E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>7.4001516683518509E-2</v>
+        <v>4.5889231757930013E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>3.6839726852567922E-2</v>
+        <v>3.3141533111534213E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>3.0323028071535418E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>-3.10187880997994E-2</v>
+        <v>2.6871287399226691E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>-3.3825356168386458E-2</v>
+        <v>2.66185913012222E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>-3.5390624053021853E-2</v>
+        <v>2.5836011005472559E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>-6.5809723300620238E-2</v>
+        <v>2.529319360808539E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>-6.6843325484947216E-2</v>
+        <v>2.331694011278911E-3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>-7.2212285249706076E-2</v>
+        <v>-6.1915905701109414E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>-7.6245577561366962E-2</v>
+        <v>-9.9630877773182643E-3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B16">
-        <v>-8.0815923207227594E-2</v>
+        <v>-2.391277166127901E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>-0.1006351732973422</v>
+        <v>-2.6344949758477499E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4566,127 +4568,127 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.1186443738263757</v>
+        <v>0.1192850049332385</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>0.1186443738263757</v>
+        <v>8.6219321473397725E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>0.11773857672492639</v>
+        <v>8.5846606859195346E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>8.3333333333333315E-2</v>
+        <v>5.501511149149229E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>7.4001516683518509E-2</v>
+        <v>5.436779794211348E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>4.2544884314913912E-2</v>
+        <v>3.2645308547359503E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>-4.1888216732261979E-2</v>
+        <v>3.0177753465087331E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>-4.1955437469199518E-2</v>
+        <v>2.707413393893748E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>-4.6397075665924978E-2</v>
+        <v>2.647331669477411E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>-6.2499999999999931E-2</v>
+        <v>2.615795458991961E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>-8.0815923207227608E-2</v>
+        <v>2.514791900163731E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>-8.5712897049947792E-2</v>
+        <v>1.9719093934636389E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>-8.6779551744993216E-2</v>
+        <v>7.798808515981105E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>-0.1006358214638059</v>
+        <v>6.384102947268714E-3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16">
-        <v>-0.10597376026755589</v>
+        <v>-2.376749705483092E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>-0.1078459910045637</v>
+        <v>-2.5075885464366E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4709,130 +4711,130 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0.19053786763942079</v>
+        <v>0.15117811022921029</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>0.1186443738263757</v>
+        <v>0.12764493441104829</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>0.1186443738263757</v>
+        <v>0.102951830941775</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>0.11773857672492639</v>
+        <v>7.2721917255088184E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>8.3333333333333315E-2</v>
+        <v>6.1068996640503359E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>7.4001516683518509E-2</v>
+        <v>6.074726261380483E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>3.2679683622090727E-2</v>
+        <v>6.0122802581596253E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>-6.0371980159845781E-2</v>
+        <v>5.898478021501867E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>-6.2499999999999931E-2</v>
+        <v>2.9617383914461091E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>-6.7744252166304753E-2</v>
+        <v>2.9058907106314539E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>-7.5897996215935778E-2</v>
+        <v>1.263879257079299E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>-8.0815923207227608E-2</v>
+        <v>-1.4115593292827119E-3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>-0.1006358214638059</v>
+        <v>-4.7651760243542767E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>-0.10859163228190601</v>
+        <v>-8.1821325816319561E-3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>-0.10992342336573729</v>
+        <v>-1.276246224460818E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>-0.1149854421878314</v>
+        <v>-5.775035826821226E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>